<commit_message>
Working file with executing using pom.xml
</commit_message>
<xml_diff>
--- a/target/classes/testdata1.xlsx
+++ b/target/classes/testdata1.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/edd665445ed33d38/Documents/_Shanthi_Learn/Team2_TaxExempt-master/Team2_TaxExempt-master/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:801_{AA50D8B6-0412-4352-8FD1-2DB33CBED647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B34B3DB1-D3A1-4B16-9919-FD84B8DAA0F1}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:801_{AA50D8B6-0412-4352-8FD1-2DB33CBED647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{11917906-7C7D-493D-A374-C1A64CE2588B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t>TCID</t>
   </si>
@@ -93,12 +94,6 @@
     <t>TC3</t>
   </si>
   <si>
-    <t>Submit A Request with invalid Request Type</t>
-  </si>
-  <si>
-    <t>I want to return this product</t>
-  </si>
-  <si>
     <t>ordernumber</t>
   </si>
   <si>
@@ -123,9 +118,6 @@
     <t>TC6</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify the Required fields </t>
-  </si>
-  <si>
     <t>abc</t>
   </si>
   <si>
@@ -189,40 +181,73 @@
     <t>abd</t>
   </si>
   <si>
-    <t>Verify different password</t>
-  </si>
-  <si>
-    <t>Birkey</t>
-  </si>
-  <si>
-    <t>Lors</t>
-  </si>
-  <si>
-    <t>a2b@gmailc.om</t>
+    <t>Verify all the fields with numbers</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Number of Test cases </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of Automated Scripts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of test cases failed </t>
+  </si>
+  <si>
+    <t>Number of test cases passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defects </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In firstname and last name taking single characters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">first name and last name taking single numbers </t>
   </si>
   <si>
     <t>TC7</t>
   </si>
   <si>
-    <t>Verify all the fields with numbers</t>
+    <t xml:space="preserve">verify all the fields with numbers </t>
   </si>
   <si>
     <t>TC8</t>
   </si>
   <si>
-    <t>Verify first and last name field with minimum characters</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>kl@gmail.com</t>
-  </si>
-  <si>
-    <t>kl</t>
+    <t>123asdertfffm34557</t>
+  </si>
+  <si>
+    <t>verify email field with numbers and chracters</t>
+  </si>
+  <si>
+    <t>TC9</t>
+  </si>
+  <si>
+    <t>Verify password fields with different passwords</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>def@gmail.com</t>
+  </si>
+  <si>
+    <t>jkl</t>
+  </si>
+  <si>
+    <t>lkj</t>
+  </si>
+  <si>
+    <t>password field is taking more number of characters</t>
+  </si>
+  <si>
+    <t>If we numbers and characters in the email field some times it was not giving error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone number is accepting single number . </t>
   </si>
 </sst>
 </file>
@@ -704,15 +729,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="48.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" customWidth="1"/>
     <col min="5" max="5" width="31.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
@@ -730,22 +756,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -753,19 +779,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <v>400500600</v>
@@ -782,7 +808,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -793,59 +819,59 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
         <v>46</v>
       </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>49</v>
-      </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G6">
         <v>456</v>
@@ -859,89 +885,168 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" t="s">
-        <v>58</v>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>3004005000</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2343</v>
       </c>
       <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="I8">
-        <v>5</v>
+        <v>34353</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
-        <v>63</v>
-      </c>
       <c r="E9" t="s">
         <v>64</v>
       </c>
-      <c r="F9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9">
-        <v>9008003000</v>
-      </c>
-      <c r="H9" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I9" t="s">
-        <v>66</v>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10">
+        <v>3345678901</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{6AA89BF0-551A-468A-AA0A-138F596DC9EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5437AD42-7F73-47DC-841B-CC8F84EAEA70}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -949,12 +1054,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -992,7 +1097,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>12</v>
@@ -1061,24 +1166,26 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="9">
         <v>8986788967</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="9">
-        <v>65478</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>24</v>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4">
+        <v>4568</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1089,25 +1196,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="9">
-        <v>8986788967</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5">
-        <v>4568</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1118,40 +1213,17 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="7">
-        <v>8090900890</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F6" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{CE709DE5-98DC-43BE-8E74-8913E8914E2B}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{1AB8AE0A-8FD4-4043-8AE1-3526DBDDBEB0}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{AC928836-1A4F-4E67-B4A1-EE6FEC5DA726}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{D1298044-FE63-49A3-85C8-96A60CE1C5A5}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{F4318CA4-A520-4883-A19A-9C62440F9E0A}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{AD18930C-A7EB-4CB7-99EE-CF4B5B3DC8A0}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{D1298044-FE63-49A3-85C8-96A60CE1C5A5}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{F4318CA4-A520-4883-A19A-9C62440F9E0A}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{18164F6A-69D4-475A-A09E-494DE05609DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>